<commit_message>
Update code to reflect changes made in excel template
</commit_message>
<xml_diff>
--- a/excelTemplate/template.xlsx
+++ b/excelTemplate/template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezepi\Documents\GitHub Repositories\ithTimesheetAutomation\excelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D149B248-2DF0-43FE-ACD4-0184143665A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5C302A-045C-4196-AA6D-5CD55043C5EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -65,12 +66,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Hrs Worked</t>
-  </si>
-  <si>
-    <t>From - To</t>
-  </si>
-  <si>
     <t>Mon</t>
   </si>
   <si>
@@ -89,40 +84,46 @@
     <t>Sun</t>
   </si>
   <si>
+    <t>Annual Leave To Be Paid = Enter Hours</t>
+  </si>
+  <si>
+    <t>International Tier 4 students declaration (required for Tier 4s only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee Use Only (must be completed by every employee) </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>1) I declare that the hours claimed, including any paid annual leave, are a true and accurate account of my hours worked.</t>
+  </si>
+  <si>
+    <t>2) I declare that I have not worked more than my restricted hours across all paid and unpaid employment. I understand breaches will be reported to UKVI</t>
+  </si>
+  <si>
+    <t>PLEASE TICK BELOW</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Cost Centre(s)</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total Hrs </t>
   </si>
   <si>
-    <t>Annual Leave To Be Paid = Enter Hours</t>
-  </si>
-  <si>
-    <t>International Tier 4 students declaration (required for Tier 4s only)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee Use Only (must be completed by every employee) </t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>1) I declare that the hours claimed, including any paid annual leave, are a true and accurate account of my hours worked.</t>
-  </si>
-  <si>
-    <t>2) I declare that I have not worked more than my restricted hours across all paid and unpaid employment. I understand breaches will be reported to UKVI</t>
-  </si>
-  <si>
-    <t>PLEASE TICK BELOW</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Cost Centre(s)</t>
-  </si>
-  <si>
-    <t>Wed</t>
-  </si>
-  <si>
-    <t>Information Service</t>
+    <t>Hrs Worked less breaks (From - To)</t>
+  </si>
+  <si>
+    <t>Enter as 00:00 (use 24 hr clock)</t>
+  </si>
+  <si>
+    <t>IS</t>
   </si>
 </sst>
 </file>
@@ -132,7 +133,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -640,13 +641,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -677,9 +671,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -691,29 +682,152 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -721,54 +835,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -783,13 +849,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -810,14 +876,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -850,75 +908,27 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1196,279 +1206,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:AN47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
-    <col min="4" max="7" width="14.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="21" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="2"/>
-    <col min="13" max="13" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="2" customWidth="1"/>
+    <col min="4" max="7" width="14.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" style="49"/>
+    <col min="14" max="14" width="9.81640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="15" max="25" width="9.1796875" style="49"/>
+    <col min="26" max="40" width="9.1796875" style="35"/>
+    <col min="41" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:14" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="93"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="39"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="3"/>
+      <c r="M1" s="48"/>
+    </row>
+    <row r="2" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="32"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="32" t="s">
+      <c r="M2" s="50"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="35" t="s">
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="35" t="s">
+      <c r="F3" s="103"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="38"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="4"/>
-      <c r="P4" s="43"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="33" t="s">
+      <c r="K3" s="36"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="31"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="84" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="105"/>
+      <c r="E5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="35" t="s">
+      <c r="F5" s="103"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="45"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="75" t="s">
+      <c r="K5" s="37"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="31"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="97"/>
+      <c r="C7" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="91" t="s">
+      <c r="D7" s="108" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="109"/>
+      <c r="F7" s="108" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="109"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="112" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="88"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="98"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="111"/>
+      <c r="F8" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="111"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="106"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="91" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="92"/>
-      <c r="H7" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="67"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A8" s="77"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="93" t="s">
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="41">
+        <f>SUM(E9-D9)+(G9-F9)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="45">
+        <f>HOUR(H9)+MINUTE(H9)/60</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="81">
+        <v>47008</v>
+      </c>
+      <c r="K9" s="82"/>
+    </row>
+    <row r="10" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="85"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="94"/>
-      <c r="F8" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="94"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="87"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="7" t="s">
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="41">
+        <f>SUM(E10-D10)+(G10-F10)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="46">
+        <f>HOUR(H10)+MINUTE(H10)/60</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="81">
+        <v>47008</v>
+      </c>
+      <c r="K10" s="82"/>
+      <c r="N10" s="51"/>
+    </row>
+    <row r="11" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="85"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="67"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="41">
+        <f t="shared" ref="H11:H15" si="0">SUM(E11-D11)+(G11-F11)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="46">
+        <f t="shared" ref="I11:I15" si="1">HOUR(H11)+MINUTE(H11)/60</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="81">
+        <v>47008</v>
+      </c>
+      <c r="K11" s="82"/>
+    </row>
+    <row r="12" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="85"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="101">
+      <c r="D12" s="67"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="81">
         <v>47008</v>
       </c>
-      <c r="J9" s="102"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="89"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="8" t="s">
+      <c r="K12" s="82"/>
+    </row>
+    <row r="13" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="89">
+      <c r="D13" s="69"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="81">
         <v>47008</v>
       </c>
-      <c r="J10" s="90"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="89"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52">
+      <c r="K13" s="82"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A14" s="79"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="71"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="81">
         <v>47008</v>
       </c>
-      <c r="J11" s="53"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="89"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="52">
+      <c r="K14" s="82"/>
+    </row>
+    <row r="15" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="73"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="73">
         <v>47008</v>
       </c>
-      <c r="J12" s="53"/>
-    </row>
-    <row r="13" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A13" s="79"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="79">
-        <v>47008</v>
-      </c>
-      <c r="J13" s="80"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="99"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="103">
-        <v>47008</v>
-      </c>
-      <c r="J14" s="104"/>
-    </row>
-    <row r="15" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A15" s="79"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="79">
-        <v>47008</v>
-      </c>
-      <c r="J15" s="80"/>
-    </row>
-    <row r="16" spans="1:16" ht="19.5" thickBot="1">
+      <c r="K15" s="74"/>
+    </row>
+    <row r="16" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="6"/>
       <c r="B16" s="14"/>
       <c r="C16" s="13"/>
@@ -1476,151 +1546,485 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="12">
-        <f>SUM(H9:H15)</f>
+      <c r="H16" s="14"/>
+      <c r="I16" s="12">
+        <f>SUM(I9:I15)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="95"/>
-      <c r="J16" s="96"/>
-    </row>
-    <row r="17" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="105" t="s">
+      <c r="J16" s="75"/>
+      <c r="K16" s="76"/>
+    </row>
+    <row r="17" spans="1:15" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="34"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="38">
+        <v>0</v>
+      </c>
+      <c r="J17" s="77"/>
+      <c r="K17" s="78"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="52"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A19" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="63">
-        <v>0</v>
-      </c>
-      <c r="I17" s="97"/>
-      <c r="J17" s="98"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" thickBot="1">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="15" t="s">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A21" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="1:15" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="25"/>
-      <c r="K20" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="25"/>
-    </row>
-    <row r="22" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A22" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="26"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23" s="53"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24" s="53"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A25" s="53"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A26" s="53"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A27" s="53"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A28" s="53"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A29" s="53"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A30" s="53"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A31" s="53"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A32" s="53"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" s="53"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" s="53"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="53"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="53"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="53"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" s="53"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39" s="53"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40" s="53"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41" s="53"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42" s="53"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43" s="53"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="53"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" s="53"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="53"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47" s="53"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Ee0zD2pVR2mQuXIylrGiCcRtgiDt3EnvxCKUYf/3Ni2Te/tC8dSUqgbUk7yQ7HFNvvJ1QOeS5STV3+sKxz8Clg==" saltValue="Q9GL9UMiBDFv8/AEf177Pg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
-  <mergeCells count="28">
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="I7:J8"/>
-    <mergeCell ref="A1:J1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7EurgSV3PjeyAyNNBddHNG6dOA7tIhY7JbDsamiNDuvQifw+Z112uvjMypn5/mb7qOfgNE1zEu4Gxn6zGKUP7A==" saltValue="W4I8VZJlW7u66P5lTtNUzQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <mergeCells count="30">
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A7:B8"/>
-    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="J13:K13"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F3:I3"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F5:I5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I22" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$K$19:$K$20</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J22" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>$L$19:$L$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$K$17:$K$18</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J20" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>$L$17:$L$18</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>

</xml_diff>